<commit_message>
1. records nand write and host write size. 2. g_nand_write_size++ in ftl_update_table_P2L function. 3. g_nand_write_size++ in ftl_garbage_collection_new function for move valid page data to GC target. 4. g_host_write_size++ in ftl_write_data_flow function for write every one page write. 5. Add ftl_write_waf_record_to_csv function for display plot chart.
</commit_message>
<xml_diff>
--- a/Document/Pages_Calc.xlsx
+++ b/Document/Pages_Calc.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="69">
   <si>
     <t>TOTAL_DIES</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -279,6 +279,10 @@
   </si>
   <si>
     <t>USED_VB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRIGGER_GC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -822,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L7"/>
+  <dimension ref="B1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -840,12 +844,13 @@
     <col min="8" max="8" width="5.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="21.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
@@ -871,13 +876,16 @@
         <v>66</v>
       </c>
       <c r="K2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="M2" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -907,15 +915,18 @@
         <v>32</v>
       </c>
       <c r="K3" s="10">
+        <v>9</v>
+      </c>
+      <c r="L3" s="10">
         <f>C7-C6*2-H3</f>
         <v>369</v>
       </c>
-      <c r="L3" s="6">
+      <c r="M3" s="6">
         <f>ROUNDUP(F3,0)</f>
         <v>5608</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -944,16 +955,19 @@
         <f>C4-I4</f>
         <v>109</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="10">
+        <v>9</v>
+      </c>
+      <c r="L4" s="11">
         <f>C7-C6*2-H4</f>
         <v>1289</v>
       </c>
-      <c r="L4" s="2">
-        <f t="shared" ref="L4:L7" si="1">ROUNDUP(F4,0)</f>
+      <c r="M4" s="2">
+        <f t="shared" ref="M4:M7" si="1">ROUNDUP(F4,0)</f>
         <v>4688</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -982,16 +996,19 @@
         <f>C4-I5</f>
         <v>61</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="10">
+        <v>9</v>
+      </c>
+      <c r="L5" s="11">
         <f>C7-C6*2-H5</f>
         <v>713</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <f t="shared" si="1"/>
         <v>5264</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1021,16 +1038,19 @@
         <f>C4-I6</f>
         <v>129</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="10">
+        <v>9</v>
+      </c>
+      <c r="L6" s="11">
         <f>C7-C6*2-H6</f>
         <v>1532</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <f t="shared" si="1"/>
         <v>4445</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1061,10 +1081,13 @@
         <v>147</v>
       </c>
       <c r="K7" s="12">
+        <v>9</v>
+      </c>
+      <c r="L7" s="12">
         <f>C7-C6*2-H7</f>
         <v>1751</v>
       </c>
-      <c r="L7" s="4">
+      <c r="M7" s="4">
         <f t="shared" si="1"/>
         <v>4226</v>
       </c>

</xml_diff>